<commit_message>
completed 2-5, need 1,6
</commit_message>
<xml_diff>
--- a/Homework1/results.xlsx
+++ b/Homework1/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke/dev/school/ALGO/Homework1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lchan\dev\school\CSE5350\Homework1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2559AB-041A-4B47-8A42-0038BD1CF79E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{46442B34-FDB6-4A72-BB6B-25FA3581FF8C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,30 +19,6 @@
     <sheet name="QuickSort" sheetId="4" r:id="rId4"/>
     <sheet name="Combined" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.10" hidden="1">Combined!$C$27:$C$28</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Combined!$C$29:$C$38</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Combined!$A$29:$A$38</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Combined!$B$27:$B$28</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Combined!$B$29:$B$38</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Combined!$C$27:$C$28</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Combined!$C$29:$C$38</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Combined!$A$29:$A$38</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Combined!$B$27:$B$28</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Combined!$B$29:$B$38</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Combined!$C$27:$C$28</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Combined!$C$29:$C$38</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Combined!$A$27:$A$28</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Combined!$A$29:$A$38</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Combined!$B$27:$B$28</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Combined!$B$29:$B$38</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Combined!$A$27:$A$28</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Combined!$A$29:$A$38</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Combined!$B$27:$B$28</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Combined!$B$29:$B$38</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Combined!$C$27:$C$28</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Combined!$C$29:$C$38</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -5710,14 +5686,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -5746,16 +5722,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>835025</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>263525</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6086,20 +6062,20 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6107,7 +6083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6145,7 +6121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10000000</v>
       </c>
@@ -6183,7 +6159,7 @@
         <v>1000742</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20000000</v>
       </c>
@@ -6221,7 +6197,7 @@
         <v>2002497</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30000000</v>
       </c>
@@ -6259,7 +6235,7 @@
         <v>2996599</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40000000</v>
       </c>
@@ -6297,7 +6273,7 @@
         <v>4000016</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50000000</v>
       </c>
@@ -6335,7 +6311,7 @@
         <v>5001463</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>60000000</v>
       </c>
@@ -6373,7 +6349,7 @@
         <v>6003106</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>70000000</v>
       </c>
@@ -6411,7 +6387,7 @@
         <v>7003426</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>80000000</v>
       </c>
@@ -6449,7 +6425,7 @@
         <v>8001300</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>90000000</v>
       </c>
@@ -6487,7 +6463,7 @@
         <v>9001735</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100000000</v>
       </c>
@@ -6525,7 +6501,7 @@
         <v>9998732</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -6533,7 +6509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -6571,7 +6547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10000</v>
       </c>
@@ -6609,7 +6585,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20000</v>
       </c>
@@ -6647,7 +6623,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>30000</v>
       </c>
@@ -6685,7 +6661,7 @@
         <v>2990</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>40000</v>
       </c>
@@ -6723,7 +6699,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>50000</v>
       </c>
@@ -6761,7 +6737,7 @@
         <v>4932</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>60000</v>
       </c>
@@ -6799,7 +6775,7 @@
         <v>5884</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>70000</v>
       </c>
@@ -6837,7 +6813,7 @@
         <v>6960</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>80000</v>
       </c>
@@ -6875,7 +6851,7 @@
         <v>8029</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>90000</v>
       </c>
@@ -6913,7 +6889,7 @@
         <v>9025</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>100000</v>
       </c>
@@ -6951,7 +6927,7 @@
         <v>10089</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -6959,7 +6935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -6997,7 +6973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10000</v>
       </c>
@@ -7035,7 +7011,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20000</v>
       </c>
@@ -7073,7 +7049,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>30000</v>
       </c>
@@ -7111,7 +7087,7 @@
         <v>2929</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>40000</v>
       </c>
@@ -7149,7 +7125,7 @@
         <v>4047</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>50000</v>
       </c>
@@ -7187,7 +7163,7 @@
         <v>5138</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>60000</v>
       </c>
@@ -7225,7 +7201,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>70000</v>
       </c>
@@ -7263,7 +7239,7 @@
         <v>7222</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>80000</v>
       </c>
@@ -7301,7 +7277,7 @@
         <v>8015</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>90000</v>
       </c>
@@ -7339,7 +7315,7 @@
         <v>9044</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>100000</v>
       </c>
@@ -7390,9 +7366,9 @@
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -7400,7 +7376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10000000</v>
       </c>
@@ -7408,7 +7384,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20000000</v>
       </c>
@@ -7416,7 +7392,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30000000</v>
       </c>
@@ -7424,7 +7400,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40000000</v>
       </c>
@@ -7432,7 +7408,7 @@
         <v>2137</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50000000</v>
       </c>
@@ -7440,7 +7416,7 @@
         <v>2682</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60000000</v>
       </c>
@@ -7448,7 +7424,7 @@
         <v>3305</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>70000000</v>
       </c>
@@ -7456,7 +7432,7 @@
         <v>3865</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80000000</v>
       </c>
@@ -7464,7 +7440,7 @@
         <v>4455</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90000000</v>
       </c>
@@ -7472,7 +7448,7 @@
         <v>5424</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100000000</v>
       </c>
@@ -7494,9 +7470,9 @@
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -7504,7 +7480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -7512,7 +7488,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20000</v>
       </c>
@@ -7520,7 +7496,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30000</v>
       </c>
@@ -7528,7 +7504,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40000</v>
       </c>
@@ -7536,7 +7512,7 @@
         <v>3819</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50000</v>
       </c>
@@ -7544,7 +7520,7 @@
         <v>6099</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60000</v>
       </c>
@@ -7552,7 +7528,7 @@
         <v>8910</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>70000</v>
       </c>
@@ -7560,7 +7536,7 @@
         <v>11910</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80000</v>
       </c>
@@ -7568,7 +7544,7 @@
         <v>15721</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90000</v>
       </c>
@@ -7576,7 +7552,7 @@
         <v>19523</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100000</v>
       </c>
@@ -7598,9 +7574,9 @@
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -7608,7 +7584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -7616,7 +7592,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20000</v>
       </c>
@@ -7624,7 +7600,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30000</v>
       </c>
@@ -7632,7 +7608,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40000</v>
       </c>
@@ -7640,7 +7616,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50000</v>
       </c>
@@ -7648,7 +7624,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60000</v>
       </c>
@@ -7656,7 +7632,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>70000</v>
       </c>
@@ -7664,7 +7640,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80000</v>
       </c>
@@ -7672,7 +7648,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90000</v>
       </c>
@@ -7680,7 +7656,7 @@
         <v>2666</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100000</v>
       </c>
@@ -7698,18 +7674,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDB777E-FC97-924F-AF96-4220E64DFC66}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7717,7 +7693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10000000</v>
       </c>
@@ -7725,7 +7701,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20000000</v>
       </c>
@@ -7733,7 +7709,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30000000</v>
       </c>
@@ -7741,7 +7717,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40000000</v>
       </c>
@@ -7749,7 +7725,7 @@
         <v>2137</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50000000</v>
       </c>
@@ -7757,7 +7733,7 @@
         <v>2682</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>60000000</v>
       </c>
@@ -7765,7 +7741,7 @@
         <v>3305</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>70000000</v>
       </c>
@@ -7773,7 +7749,7 @@
         <v>3865</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>80000000</v>
       </c>
@@ -7781,7 +7757,7 @@
         <v>4455</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>90000000</v>
       </c>
@@ -7789,7 +7765,7 @@
         <v>5424</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100000000</v>
       </c>
@@ -7797,7 +7773,7 @@
         <v>5198</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>8</v>
       </c>
@@ -7805,7 +7781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -7816,7 +7792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10000</v>
       </c>
@@ -7827,7 +7803,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20000</v>
       </c>
@@ -7838,7 +7814,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30000</v>
       </c>
@@ -7849,7 +7825,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>40000</v>
       </c>
@@ -7860,7 +7836,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>50000</v>
       </c>
@@ -7871,7 +7847,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>60000</v>
       </c>
@@ -7882,7 +7858,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>70000</v>
       </c>
@@ -7893,7 +7869,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>80000</v>
       </c>
@@ -7904,7 +7880,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>90000</v>
       </c>
@@ -7915,7 +7891,7 @@
         <v>2666</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>100000</v>
       </c>

</xml_diff>